<commit_message>
Adicionado a função de salvar um arquivo excel com a lista de itens cadastrados. Também foi adicionado uma verificação se o item já esta cadastrado.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,6 +20,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -66,7 +67,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -443,223 +450,672 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="21.99" customWidth="1" style="1" min="1" max="1"/>
-    <col width="23.66" customWidth="1" style="1" min="2" max="2"/>
-    <col width="11.16" customWidth="1" style="1" min="3" max="3"/>
-    <col width="9.77" customWidth="1" style="1" min="4" max="4"/>
-    <col width="5.04" customWidth="1" style="1" min="5" max="5"/>
-    <col width="13.52" customWidth="1" style="1" min="6" max="6"/>
-    <col width="12.13" customWidth="1" style="1" min="7" max="7"/>
-    <col width="4.63" customWidth="1" style="1" min="8" max="8"/>
-    <col width="6.85" customWidth="1" style="1" min="9" max="9"/>
-    <col width="13.1" customWidth="1" style="1" min="10" max="10"/>
-    <col width="12.13" customWidth="1" style="1" min="11" max="11"/>
-    <col width="4.63" customWidth="1" style="1" min="12" max="12"/>
+    <col width="76.92" customWidth="1" style="3" min="1" max="1"/>
+    <col width="12.88" customWidth="1" style="3" min="2" max="3"/>
+    <col width="9.779999999999999" customWidth="1" style="3" min="4" max="4"/>
+    <col width="5.04" customWidth="1" style="3" min="5" max="5"/>
+    <col width="13.52" customWidth="1" style="3" min="6" max="6"/>
+    <col width="12.13" customWidth="1" style="3" min="7" max="7"/>
+    <col width="4.63" customWidth="1" style="3" min="8" max="8"/>
+    <col width="6.85" customWidth="1" style="3" min="9" max="9"/>
+    <col width="13.1" customWidth="1" style="3" min="10" max="10"/>
+    <col width="12.13" customWidth="1" style="3" min="11" max="11"/>
+    <col width="4.63" customWidth="1" style="3" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="2">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Descriçăo;Custo;Unidade</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>2.ACE.ABR.0001</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>ABRACADEIRADE</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>NYLON</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>NATURAL</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>283</v>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>4,8MM</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>(LF</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>SILVEIRA);R$</t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>25.3;Unidade</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>(un)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="12.8" customHeight="1" s="2">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>2.ACE.ABR.0002</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>ABRACADEIRADE</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>NYLON</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
-        <is>
-          <t>NATURAL</t>
-        </is>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>3,8MM</t>
-        </is>
-      </c>
-      <c r="H3" s="1" t="inlineStr">
-        <is>
-          <t>(FG</t>
-        </is>
-      </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>27);R$</t>
-        </is>
-      </c>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t>10.9;Unidade</t>
-        </is>
-      </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>(un)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="12.8" customHeight="1" s="2">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>2.ACE.ABR.0003</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>ABRACADEIRAMETALICA</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>DIAMETRO</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>-108</v>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>(SUPRIND);R$</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>3.76;Unidade</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>(un)</t>
+    <row r="1" ht="12.8" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Descriçăo</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Custo</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Unidade</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="12.8" customHeight="1" s="4">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0001 ABRACADEIRADE NYLON NATURAL 283 X 4,8MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0001 ABRACADEIRADE NYLON NATURAL 283 X 4,8MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0001 ABRACADEIRADE NYLON NATURAL 283 X 4,8MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Categoria</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Valor</t>
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0002 ABRACADEIRADE NYLON NATURAL 150 X 3,8MM (FG 27)</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Restaurante</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>45.99</v>
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0003 ABRACADEIRAMETALICA DIAMETRO 89 -108 (SUPRIND)</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Transporte</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>208.45</v>
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0004 ABRACADEIRAPARA LAMPADA FLUORECENTE (CELETRO)</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Viagem</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>558.54</v>
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0005 ABRACADEIRADE ACO NR 12-16 - MARCA FLEXIL SUPRENS (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0006 ABRACADEIRADE ACO NR 13-19 - MARCA FLEXIL SUPRENS (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0007 ABRACADEIRADE ACO 57 - 70MM (SUPRIND)</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>4.206</v>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0008 ABRACADEIRAMETALICA DIAMETRO 241 - 260MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0009 ABRACADEIRAMETALICA DIAMETRO 140 - 159MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0010 ABRACADEIRADE NYLON PRETA 536 X 13,7 PCT C/ 50PCS (FATI FERRAME)</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>119.95</v>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0011 ABRACADEIRADE NYLON NATURAL 108 X 2,5 MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0012 ABRACADEIRAINSULOK 300 X 5,0MM NYLON 6.6 NATURAL (REAL CENTER)</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>23.01</v>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0013 ABRACADEIRAINSULOK 151 X 3,7MM NYLON 6.6 NATURAL (REAL CENTER)</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>9.550000000000001</v>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0014 ABRACADEIRATIPO U 1 G/E 2912100100 VONDER (FG 27)</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0015 ABRACADEIRAS FIM 70 - 89MM L14 (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0016 ABRACADEIRAAC.KSC 3MX14,5MM KIT C/3 FECHOS SUPREN/NAC KSC K (FG 27)</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0017 ABRACADEIRATIPO MS OU MANGOTINHO PARA MANGUEIRA DE AR (PCP)</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>5.83333</v>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0018 ABRACADEIRADE NYLON COR PRETA 180 X 5 MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0019 ABRACADEIRAMETALICA 32-44MM CHAVE 8MM MARCA : FLEXIL SUPREN (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0020 ABRACADEIRANYLON 283,00MM X 4,80MM NAT (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0021 ABRACADEIRADE POLIAMIDA T30R / 150 X 3,6 - MARCA HELLERMAN (DW1)</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>7.74</v>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0022 ABRACADEIRAPRETA NYLON COMP: 390MM X 7,6MM  (CELETRO)</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0024 ABRACADEIRAMSA 35-40 FITA 32MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0025 ABRACADEIRAMICRO-ACO CARBONO 9-13 FITA 9MM - SST (VULCANO)</t>
+        </is>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0026 ABRACADEIRADE NYLON NATURAL 202 X 3,7MM  (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>10.75</v>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0027 ABRACADEIRADE NYLON NATURAL 151 X 3,65MM  (DARCA02)</t>
+        </is>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0028 ABRACADEIRADE NYLON NATURAL 200 X 4,8MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0029 ABRACADEIRADE NYLON NATURAL 387 X 7,60MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0030 ABRACADEIRA DE METAL MARCA MATRIX DIAM 38 - 51MM  LARG: 14MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="C32" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0031 ABRACADEIRADE METAL 38-51 (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="C33" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0032 ABRACADEIRADE METAL 32-44 (MG MANGUEIRA)</t>
+        </is>
+      </c>
+      <c r="B34" s="3" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="C34" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0035 ABRACADEIRAMETALICA 40-60MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B35" s="3" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="C35" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0036 ABRACADEIRAMETALICA 55-75MM (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B36" s="3" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="C36" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0037 ABRACADEIRAS FIM 102 - 121MM L14 (LF  SILVEIRA)</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="C37" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0038 ABRACADEIRATIPO D 3/4" C/CHAVETA G/E LINHA PESADA S4.112 ST (FG 27)</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="C38" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0039 ABRACADEIRAPARA CANO 89-108 (MG MANGUEIRA)</t>
+        </is>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="C39" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0040 ABRACADEIRAPARA CANO 6-159-1778  (MG MANGUEIRA)</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0041 ABRACADEIRAPARA CANO 8-191-210 (MG MANGUEIRA)</t>
+        </is>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="C41" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0042 ABRACADEIRA102-121 (MG MANGUEIRA)</t>
+        </is>
+      </c>
+      <c r="B42" s="3" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="C42" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2.ACE.ABR.0045 ABRACADEIRADE FERRO 146-165 (SUPRIND)</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retirado a função 'sleep' e utilizado função do selenium que confirma o carregamento da pagina.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
@@ -3459,15 +3459,135 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" t="inlineStr">
+      <c r="A200" s="3" t="inlineStr">
         <is>
           <t>2.ACE.ANE.0049 ANEL ELASTICO 04/03/2021 (FATI FERRAME)</t>
         </is>
       </c>
-      <c r="B200" t="n">
+      <c r="B200" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="C200" t="inlineStr">
+      <c r="C200" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ANE.0050 ANEL 15/03/2021 (MAGELB)</t>
+        </is>
+      </c>
+      <c r="B201" s="3" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="C201" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ANE.0051 ANEL ORING 25X32X4,8 mm 4-012-01-0408 20/04/2021 (MTM)</t>
+        </is>
+      </c>
+      <c r="B202" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="C202" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ANE.0052 ANEL ORING 24,9X33,5X7 TYP IV 4-012-01-0608 20/04/2021 (MTM)</t>
+        </is>
+      </c>
+      <c r="B203" s="3" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="C203" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ANE.0053 QORING DE VITON ALTA TEMPERATURA 29,74X3,53 mm 4-012-02-042 20/04/2021 (MTM)</t>
+        </is>
+      </c>
+      <c r="B204" s="3" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="C204" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ANE.0054 QORING VITON VD ›29,74X3,53 FKM 70 COD HOMAG (70283) 4-012- 20/04/2021 (MTM)</t>
+        </is>
+      </c>
+      <c r="B205" s="3" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="C205" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ANE.0055 ANEL VED NILOSRING MS0 23/06/2021 (NPX SOLUCOES)</t>
+        </is>
+      </c>
+      <c r="B206" s="3" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="C206" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="3" t="inlineStr">
+        <is>
+          <t>2.ACE.ANE.0056 ANEL TRAVA 35X1,5-FST-PHR DIN 472 23/06/2021 (NPX SOLUCOES)</t>
+        </is>
+      </c>
+      <c r="B207" s="3" t="n">
+        <v>257.6</v>
+      </c>
+      <c r="C207" s="3" t="inlineStr">
+        <is>
+          <t>Unidade (un)</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2.ACE.ANE.0057 ANEL ELASTICO E-12 13/12/2021 (CRV PARAFUSO)</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>202.01</v>
+      </c>
+      <c r="C208" t="inlineStr">
         <is>
           <t>Unidade (un)</t>
         </is>

</xml_diff>